<commit_message>
update from consolidation meetings
</commit_message>
<xml_diff>
--- a/title intersections for extraction consolidation.xlsx
+++ b/title intersections for extraction consolidation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerom\Documents\projects\mde4dts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Lehner\Desktop\Repos\Paper\MDE4DTs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D658CA4A-1ABF-4CF7-83BA-A82B0AC42FBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F07AB64-7B36-4A93-BF73-C4F41AAB72B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="title_intersections" sheetId="1" r:id="rId1"/>
@@ -198,7 +198,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -329,13 +329,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -682,11 +675,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1042,268 +1034,220 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="116.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="87.44140625" customWidth="1"/>
-    <col min="4" max="4" width="51.21875" customWidth="1"/>
+    <col min="1" max="1" width="116.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="87.42578125" customWidth="1"/>
+    <col min="3" max="3" width="51.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>0</v>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
         <v>5</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>1</v>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="2" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>5</v>
-      </c>
       <c r="B7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7" t="s">
-        <v>51</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>6</v>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="3" t="s">
         <v>52</v>
       </c>
+      <c r="C8" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="D8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="C9" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="D9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" s="1" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="C10" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="D10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" s="1" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="C11" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="D11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>33</v>
       </c>
+      <c r="C12" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="D12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>36</v>
       </c>
-      <c r="D13" t="s">
+      <c r="C13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14" s="1" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D14" t="s">
+      <c r="C14" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>13</v>
-      </c>
-      <c r="B15" s="1" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>43</v>
       </c>
-      <c r="D16" t="s">
+      <c r="C16" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>15</v>
-      </c>
-      <c r="B17" s="1" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D18" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="1" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>